<commit_message>
made table comparing DE methods
</commit_message>
<xml_diff>
--- a/data/TSC genes regulated.xlsx
+++ b/data/TSC genes regulated.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sepid\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sepid\Documents\Geschwind Lab\TSC_MIA_RNAseq\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,7 +106,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -133,14 +140,71 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -151,7 +215,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1">
-      <tableStyleElement type="wholeTable" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -166,12 +230,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C22" totalsRowShown="0" headerRowCellStyle="Bad" dataCellStyle="Bad">
-  <autoFilter ref="A1:C22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C19" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:C19"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Region"/>
-    <tableColumn id="2" name="Upregulated"/>
-    <tableColumn id="3" name="Downregulated"/>
+    <tableColumn id="1" name="Region" dataDxfId="3"/>
+    <tableColumn id="2" name="Upregulated" dataDxfId="2"/>
+    <tableColumn id="3" name="Downregulated" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -474,149 +538,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
+    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>